<commit_message>
- Added credentials for SMTP and Mailgun details
</commit_message>
<xml_diff>
--- a/document/Credential/eSportColosseum - Dev.xlsx
+++ b/document/Credential/eSportColosseum - Dev.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Sr</t>
   </si>
@@ -55,13 +55,34 @@
   </si>
   <si>
     <t>DonttellAny1</t>
+  </si>
+  <si>
+    <t>Mailgun</t>
+  </si>
+  <si>
+    <t>http://www.mailgun.com/</t>
+  </si>
+  <si>
+    <t>rukmi.patel@itreeni.com</t>
+  </si>
+  <si>
+    <t>SMTP</t>
+  </si>
+  <si>
+    <t>smtp.zoho.com</t>
+  </si>
+  <si>
+    <t>info@esportcolosseum.com</t>
+  </si>
+  <si>
+    <t>info@123</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -83,6 +104,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -123,16 +151,23 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -425,17 +460,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B6:F9"/>
+  <dimension ref="B6:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="E14" sqref="E14:E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="35" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -494,14 +529,40 @@
       <c r="B9" s="1">
         <v>3</v>
       </c>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
+      <c r="C9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>15</v>
+      </c>
       <c r="F9" s="1"/>
     </row>
+    <row r="10" spans="2:6">
+      <c r="B10" s="5">
+        <v>4</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E9" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Match List & View
</commit_message>
<xml_diff>
--- a/document/Credential/eSportColosseum - Dev.xlsx
+++ b/document/Credential/eSportColosseum - Dev.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Sr</t>
   </si>
@@ -76,13 +76,25 @@
   </si>
   <si>
     <t>info@123</t>
+  </si>
+  <si>
+    <t>Putty</t>
+  </si>
+  <si>
+    <t>132.148.72.192</t>
+  </si>
+  <si>
+    <t>esc</t>
+  </si>
+  <si>
+    <t>Esc@esc123</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -172,6 +184,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -250,6 +267,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -284,6 +302,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -459,14 +478,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B6:F10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B6:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14:E15"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="35" bestFit="1" customWidth="1"/>
@@ -474,7 +493,7 @@
     <col min="6" max="6" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="2:6">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
         <v>0</v>
       </c>
@@ -491,7 +510,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="2:6">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
         <v>1</v>
       </c>
@@ -508,7 +527,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="2:6">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B8" s="1">
         <v>2</v>
       </c>
@@ -525,7 +544,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="2:6">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B9" s="1">
         <v>3</v>
       </c>
@@ -540,7 +559,7 @@
       </c>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="2:6">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" s="5">
         <v>4</v>
       </c>
@@ -555,6 +574,23 @@
       </c>
       <c r="F10" s="2" t="s">
         <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B11" s="1">
+        <v>5</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -567,24 +603,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
- Updated new credentials in excel sheet.
</commit_message>
<xml_diff>
--- a/document/Credential/eSportColosseum - Dev.xlsx
+++ b/document/Credential/eSportColosseum - Dev.xlsx
@@ -1,22 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Crendetials" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
   <si>
     <t>Sr</t>
   </si>
@@ -30,33 +28,15 @@
     <t>Password</t>
   </si>
   <si>
-    <t xml:space="preserve">Server </t>
-  </si>
-  <si>
     <t>URL</t>
   </si>
   <si>
     <t>phpmyadmin</t>
   </si>
   <si>
-    <t>192.169.166.231</t>
-  </si>
-  <si>
-    <t>devrukmi</t>
-  </si>
-  <si>
-    <t>devrukmi@123</t>
-  </si>
-  <si>
-    <t>http://192.169.166.231/phpmyadmin/</t>
-  </si>
-  <si>
     <t>root</t>
   </si>
   <si>
-    <t>DonttellAny1</t>
-  </si>
-  <si>
     <t>Mailgun</t>
   </si>
   <si>
@@ -88,13 +68,16 @@
   </si>
   <si>
     <t>Esc@esc123</t>
+  </si>
+  <si>
+    <t>http://132.148.72.192/phpmyadmin/</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -267,7 +250,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -302,7 +284,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -478,14 +459,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B6:F11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B6:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="35" bestFit="1" customWidth="1"/>
@@ -493,7 +474,7 @@
     <col min="6" max="6" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:6">
       <c r="B6" s="3" t="s">
         <v>0</v>
       </c>
@@ -501,7 +482,7 @@
         <v>1</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>2</v>
@@ -510,87 +491,70 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:6">
       <c r="B7" s="1">
         <v>1</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>4</v>
+      <c r="C7" s="5" t="s">
+        <v>14</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:6">
       <c r="B8" s="1">
         <v>2</v>
       </c>
       <c r="C8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="F8" s="2" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:6">
       <c r="B9" s="1">
         <v>3</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:6">
       <c r="B10" s="5">
         <v>4</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B11" s="1">
-        <v>5</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -600,28 +564,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>